<commit_message>
Add new file to project
</commit_message>
<xml_diff>
--- a/public/templates/attempt_card_template.xlsx
+++ b/public/templates/attempt_card_template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boudjemaa\Desktop\wppo-papaers-work\wppo-manage-file\wppo-competition\public\templates\"/>
@@ -130,7 +130,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -368,9 +368,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -392,84 +389,93 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -478,12 +484,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,14 +799,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Feuil1">
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -816,26 +816,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
@@ -846,11 +846,11 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
@@ -873,19 +873,19 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1"/>
@@ -907,22 +907,22 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42" t="s">
+      <c r="D6" s="44"/>
+      <c r="E6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42" t="s">
+      <c r="F6" s="44"/>
+      <c r="G6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -941,20 +941,20 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="40" t="s">
+      <c r="D7" s="43"/>
+      <c r="E7" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -973,22 +973,22 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="34" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="34" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="35"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1011,106 +1011,106 @@
         <v>18</v>
       </c>
       <c r="B9" s="21"/>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="44"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:24" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="37" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="35"/>
+      <c r="G10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:24" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="36" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" spans="1:24" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="38" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="21"/>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:24" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="32" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:24" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="34" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:24" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="19" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1174,6 +1174,36 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ldca6e2accdf4b44bc6f0466176963ac xmlns="01f84582-29e4-4982-ad5e-dd0b7829e18b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">World Para Powerlifting</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">f91db9fc-eff8-42c7-b149-fa2b47e1b252</TermId>
+        </TermInfo>
+      </Terms>
+    </ldca6e2accdf4b44bc6f0466176963ac>
+    <TaxCatchAll xmlns="82e9e178-5b87-4e4e-a3c8-75f2511f250b">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="01f84582-29e4-4982-ad5e-dd0b7829e18b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B0705632E00314D9623D2052ED961FA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="103873359c057afce757505bac4dfdd0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01f84582-29e4-4982-ad5e-dd0b7829e18b" xmlns:ns3="82e9e178-5b87-4e4e-a3c8-75f2511f250b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33b1bb52899143828c36c29c130e1dd8" ns2:_="" ns3:_="">
     <xsd:import namespace="01f84582-29e4-4982-ad5e-dd0b7829e18b"/>
@@ -1418,37 +1448,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ldca6e2accdf4b44bc6f0466176963ac xmlns="01f84582-29e4-4982-ad5e-dd0b7829e18b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">World Para Powerlifting</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">f91db9fc-eff8-42c7-b149-fa2b47e1b252</TermId>
-        </TermInfo>
-      </Terms>
-    </ldca6e2accdf4b44bc6f0466176963ac>
-    <TaxCatchAll xmlns="82e9e178-5b87-4e4e-a3c8-75f2511f250b">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="01f84582-29e4-4982-ad5e-dd0b7829e18b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4592527F-6021-4FFE-A3FD-36786BEE33B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="82e9e178-5b87-4e4e-a3c8-75f2511f250b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="01f84582-29e4-4982-ad5e-dd0b7829e18b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06D5460B-F0D7-4E4B-A8AA-7298828F752E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B2075C-4C9E-4C75-A4BB-558501245C59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1465,29 +1490,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4592527F-6021-4FFE-A3FD-36786BEE33B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="82e9e178-5b87-4e4e-a3c8-75f2511f250b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="01f84582-29e4-4982-ad5e-dd0b7829e18b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06D5460B-F0D7-4E4B-A8AA-7298828F752E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>